<commit_message>
Data management + analysis 11-05
</commit_message>
<xml_diff>
--- a/data_management/df_tendances_final.xlsx
+++ b/data_management/df_tendances_final.xlsx
@@ -550,10 +550,10 @@
     <t>Ibrahim Maalouf</t>
   </si>
   <si>
-    <t>[[0.38495379]]</t>
-  </si>
-  <si>
-    <t>[[0.48923893]]</t>
+    <t>[[0.23604506]]</t>
+  </si>
+  <si>
+    <t>[[0.36709314]]</t>
   </si>
 </sst>
 </file>
@@ -1080,31 +1080,31 @@
         <v>4</v>
       </c>
       <c r="V2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="X2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y2">
         <v>10</v>
       </c>
       <c r="Z2">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA2">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB2">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC2">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD2">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE2" t="s">
         <v>178</v>
@@ -1178,31 +1178,31 @@
         <v>4</v>
       </c>
       <c r="V3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="X3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y3">
         <v>10</v>
       </c>
       <c r="Z3">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA3">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB3">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC3">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD3">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE3" t="s">
         <v>178</v>
@@ -1276,31 +1276,31 @@
         <v>4</v>
       </c>
       <c r="V4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="X4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y4">
         <v>10</v>
       </c>
       <c r="Z4">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA4">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB4">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC4">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD4">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE4" t="s">
         <v>178</v>
@@ -1380,25 +1380,25 @@
         <v>6</v>
       </c>
       <c r="X5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y5">
         <v>10</v>
       </c>
       <c r="Z5">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA5">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB5">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC5">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD5">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE5" t="s">
         <v>178</v>
@@ -1472,31 +1472,31 @@
         <v>4</v>
       </c>
       <c r="V6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="X6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y6">
         <v>10</v>
       </c>
       <c r="Z6">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA6">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB6">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC6">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD6">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE6" t="s">
         <v>178</v>
@@ -1570,31 +1570,31 @@
         <v>4</v>
       </c>
       <c r="V7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="X7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y7">
         <v>10</v>
       </c>
       <c r="Z7">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA7">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB7">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC7">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD7">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE7" t="s">
         <v>178</v>
@@ -1668,31 +1668,31 @@
         <v>4</v>
       </c>
       <c r="V8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W8">
         <v>1</v>
       </c>
       <c r="X8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y8">
         <v>10</v>
       </c>
       <c r="Z8">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA8">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB8">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC8">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD8">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE8" t="s">
         <v>178</v>
@@ -1769,28 +1769,28 @@
         <v>1</v>
       </c>
       <c r="W9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y9">
         <v>10</v>
       </c>
       <c r="Z9">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA9">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB9">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC9">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD9">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE9" t="s">
         <v>178</v>
@@ -1867,28 +1867,28 @@
         <v>1</v>
       </c>
       <c r="W10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y10">
         <v>10</v>
       </c>
       <c r="Z10">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA10">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB10">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC10">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD10">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE10" t="s">
         <v>178</v>
@@ -1962,31 +1962,31 @@
         <v>4</v>
       </c>
       <c r="V11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="X11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y11">
         <v>10</v>
       </c>
       <c r="Z11">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA11">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB11">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC11">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD11">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE11" t="s">
         <v>178</v>
@@ -2066,25 +2066,25 @@
         <v>6</v>
       </c>
       <c r="X12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y12">
         <v>10</v>
       </c>
       <c r="Z12">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA12">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB12">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC12">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD12">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE12" t="s">
         <v>178</v>
@@ -2158,31 +2158,31 @@
         <v>4</v>
       </c>
       <c r="V13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W13">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="X13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y13">
         <v>10</v>
       </c>
       <c r="Z13">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA13">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB13">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC13">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD13">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE13" t="s">
         <v>178</v>
@@ -2256,31 +2256,31 @@
         <v>4</v>
       </c>
       <c r="V14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y14">
         <v>10</v>
       </c>
       <c r="Z14">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA14">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB14">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC14">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD14">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE14" t="s">
         <v>178</v>
@@ -2354,31 +2354,31 @@
         <v>4</v>
       </c>
       <c r="V15">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W15">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="X15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y15">
         <v>10</v>
       </c>
       <c r="Z15">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA15">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB15">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC15">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD15">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE15" t="s">
         <v>178</v>
@@ -2452,31 +2452,31 @@
         <v>4</v>
       </c>
       <c r="V16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y16">
         <v>10</v>
       </c>
       <c r="Z16">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA16">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB16">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC16">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD16">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE16" t="s">
         <v>178</v>
@@ -2550,31 +2550,31 @@
         <v>4</v>
       </c>
       <c r="V17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W17">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="X17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y17">
         <v>10</v>
       </c>
       <c r="Z17">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA17">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB17">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC17">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD17">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE17" t="s">
         <v>178</v>
@@ -2648,31 +2648,31 @@
         <v>4</v>
       </c>
       <c r="V18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W18">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="X18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y18">
         <v>10</v>
       </c>
       <c r="Z18">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA18">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB18">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC18">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD18">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE18" t="s">
         <v>178</v>
@@ -2746,31 +2746,31 @@
         <v>4</v>
       </c>
       <c r="V19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W19">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="X19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y19">
         <v>10</v>
       </c>
       <c r="Z19">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA19">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB19">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC19">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD19">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE19" t="s">
         <v>178</v>
@@ -2844,31 +2844,31 @@
         <v>4</v>
       </c>
       <c r="V20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="X20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y20">
         <v>10</v>
       </c>
       <c r="Z20">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA20">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB20">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC20">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD20">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE20" t="s">
         <v>178</v>
@@ -2945,28 +2945,28 @@
         <v>0</v>
       </c>
       <c r="W21">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="X21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y21">
         <v>10</v>
       </c>
       <c r="Z21">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA21">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB21">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC21">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD21">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE21" t="s">
         <v>178</v>
@@ -3043,28 +3043,28 @@
         <v>1</v>
       </c>
       <c r="W22">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="X22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y22">
         <v>10</v>
       </c>
       <c r="Z22">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA22">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB22">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC22">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD22">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE22" t="s">
         <v>178</v>
@@ -3138,31 +3138,31 @@
         <v>4</v>
       </c>
       <c r="V23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W23">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="X23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y23">
         <v>10</v>
       </c>
       <c r="Z23">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA23">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB23">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC23">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD23">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE23" t="s">
         <v>178</v>
@@ -3242,25 +3242,25 @@
         <v>6</v>
       </c>
       <c r="X24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y24">
         <v>10</v>
       </c>
       <c r="Z24">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA24">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB24">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC24">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD24">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE24" t="s">
         <v>178</v>
@@ -3340,25 +3340,25 @@
         <v>6</v>
       </c>
       <c r="X25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y25">
         <v>10</v>
       </c>
       <c r="Z25">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA25">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB25">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC25">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD25">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE25" t="s">
         <v>178</v>
@@ -3435,28 +3435,28 @@
         <v>1</v>
       </c>
       <c r="W26">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="X26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y26">
         <v>10</v>
       </c>
       <c r="Z26">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA26">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB26">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC26">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD26">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE26" t="s">
         <v>178</v>
@@ -3530,31 +3530,31 @@
         <v>4</v>
       </c>
       <c r="V27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y27">
         <v>10</v>
       </c>
       <c r="Z27">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA27">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB27">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC27">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD27">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE27" t="s">
         <v>178</v>
@@ -3631,28 +3631,28 @@
         <v>1</v>
       </c>
       <c r="W28">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="X28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y28">
         <v>10</v>
       </c>
       <c r="Z28">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA28">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB28">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC28">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD28">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE28" t="s">
         <v>178</v>
@@ -3729,28 +3729,28 @@
         <v>1</v>
       </c>
       <c r="W29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X29">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y29">
         <v>10</v>
       </c>
       <c r="Z29">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA29">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB29">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC29">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD29">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE29" t="s">
         <v>178</v>
@@ -3827,28 +3827,28 @@
         <v>1</v>
       </c>
       <c r="W30">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="X30">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y30">
         <v>10</v>
       </c>
       <c r="Z30">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA30">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB30">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC30">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD30">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE30" t="s">
         <v>178</v>
@@ -3922,31 +3922,31 @@
         <v>3</v>
       </c>
       <c r="V31">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W31">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="X31">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y31">
         <v>10</v>
       </c>
       <c r="Z31">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA31">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB31">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC31">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD31">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE31" t="s">
         <v>178</v>
@@ -4020,31 +4020,31 @@
         <v>4</v>
       </c>
       <c r="V32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W32">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="X32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y32">
         <v>10</v>
       </c>
       <c r="Z32">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA32">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB32">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC32">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD32">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE32" t="s">
         <v>178</v>
@@ -4121,28 +4121,28 @@
         <v>1</v>
       </c>
       <c r="W33">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="X33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y33">
         <v>10</v>
       </c>
       <c r="Z33">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA33">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB33">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC33">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD33">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE33" t="s">
         <v>178</v>
@@ -4216,31 +4216,31 @@
         <v>4</v>
       </c>
       <c r="V34">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="X34">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y34">
         <v>10</v>
       </c>
       <c r="Z34">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA34">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB34">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC34">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD34">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE34" t="s">
         <v>178</v>
@@ -4314,31 +4314,31 @@
         <v>4</v>
       </c>
       <c r="V35">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W35">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="X35">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y35">
         <v>10</v>
       </c>
       <c r="Z35">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA35">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB35">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC35">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD35">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE35" t="s">
         <v>178</v>
@@ -4415,28 +4415,28 @@
         <v>1</v>
       </c>
       <c r="W36">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="X36">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y36">
         <v>10</v>
       </c>
       <c r="Z36">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA36">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB36">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC36">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD36">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE36" t="s">
         <v>178</v>
@@ -4510,31 +4510,31 @@
         <v>4</v>
       </c>
       <c r="V37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W37">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="X37">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y37">
         <v>10</v>
       </c>
       <c r="Z37">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA37">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB37">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC37">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD37">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE37" t="s">
         <v>178</v>
@@ -4608,31 +4608,31 @@
         <v>4</v>
       </c>
       <c r="V38">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W38">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="X38">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y38">
         <v>10</v>
       </c>
       <c r="Z38">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA38">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB38">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC38">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD38">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE38" t="s">
         <v>178</v>
@@ -4706,31 +4706,31 @@
         <v>4</v>
       </c>
       <c r="V39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W39">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="X39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y39">
         <v>10</v>
       </c>
       <c r="Z39">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA39">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB39">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC39">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD39">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE39" t="s">
         <v>178</v>
@@ -4804,31 +4804,31 @@
         <v>4</v>
       </c>
       <c r="V40">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W40">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="X40">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y40">
         <v>10</v>
       </c>
       <c r="Z40">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA40">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB40">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC40">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD40">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE40" t="s">
         <v>178</v>
@@ -4905,28 +4905,28 @@
         <v>1</v>
       </c>
       <c r="W41">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="X41">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y41">
         <v>10</v>
       </c>
       <c r="Z41">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA41">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB41">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC41">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD41">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE41" t="s">
         <v>178</v>
@@ -5003,28 +5003,28 @@
         <v>1</v>
       </c>
       <c r="W42">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="X42">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y42">
         <v>10</v>
       </c>
       <c r="Z42">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA42">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB42">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC42">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD42">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE42" t="s">
         <v>178</v>
@@ -5098,31 +5098,31 @@
         <v>4</v>
       </c>
       <c r="V43">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W43">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="X43">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y43">
         <v>10</v>
       </c>
       <c r="Z43">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA43">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB43">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC43">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD43">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE43" t="s">
         <v>178</v>
@@ -5196,31 +5196,31 @@
         <v>4</v>
       </c>
       <c r="V44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W44">
         <v>3</v>
       </c>
       <c r="X44">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y44">
         <v>10</v>
       </c>
       <c r="Z44">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA44">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB44">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC44">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD44">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE44" t="s">
         <v>178</v>
@@ -5294,31 +5294,31 @@
         <v>4</v>
       </c>
       <c r="V45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W45">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="X45">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y45">
         <v>10</v>
       </c>
       <c r="Z45">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA45">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB45">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC45">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD45">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE45" t="s">
         <v>178</v>
@@ -5392,31 +5392,31 @@
         <v>4</v>
       </c>
       <c r="V46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W46">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="X46">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y46">
         <v>10</v>
       </c>
       <c r="Z46">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA46">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB46">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC46">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD46">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE46" t="s">
         <v>178</v>
@@ -5490,31 +5490,31 @@
         <v>4</v>
       </c>
       <c r="V47">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W47">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="X47">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y47">
         <v>10</v>
       </c>
       <c r="Z47">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA47">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB47">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC47">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD47">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE47" t="s">
         <v>178</v>
@@ -5588,31 +5588,31 @@
         <v>4</v>
       </c>
       <c r="V48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W48">
         <v>1</v>
       </c>
       <c r="X48">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y48">
         <v>10</v>
       </c>
       <c r="Z48">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA48">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB48">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC48">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD48">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE48" t="s">
         <v>178</v>
@@ -5686,31 +5686,31 @@
         <v>4</v>
       </c>
       <c r="V49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W49">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="X49">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y49">
         <v>10</v>
       </c>
       <c r="Z49">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA49">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB49">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC49">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD49">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE49" t="s">
         <v>178</v>
@@ -5787,28 +5787,28 @@
         <v>1</v>
       </c>
       <c r="W50">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="X50">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y50">
         <v>10</v>
       </c>
       <c r="Z50">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA50">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB50">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC50">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD50">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE50" t="s">
         <v>178</v>
@@ -5882,31 +5882,31 @@
         <v>4</v>
       </c>
       <c r="V51">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W51">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="X51">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y51">
         <v>10</v>
       </c>
       <c r="Z51">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA51">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB51">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC51">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD51">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE51" t="s">
         <v>178</v>
@@ -5983,28 +5983,28 @@
         <v>1</v>
       </c>
       <c r="W52">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="X52">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y52">
         <v>10</v>
       </c>
       <c r="Z52">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA52">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB52">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC52">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD52">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE52" t="s">
         <v>178</v>
@@ -6081,28 +6081,28 @@
         <v>1</v>
       </c>
       <c r="W53">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="X53">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y53">
         <v>10</v>
       </c>
       <c r="Z53">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA53">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB53">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC53">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD53">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE53" t="s">
         <v>178</v>
@@ -6179,28 +6179,28 @@
         <v>0</v>
       </c>
       <c r="W54">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="X54">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y54">
         <v>10</v>
       </c>
       <c r="Z54">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA54">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB54">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC54">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD54">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE54" t="s">
         <v>178</v>
@@ -6274,31 +6274,31 @@
         <v>4</v>
       </c>
       <c r="V55">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W55">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="X55">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y55">
         <v>10</v>
       </c>
       <c r="Z55">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA55">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB55">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC55">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD55">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE55" t="s">
         <v>178</v>
@@ -6372,31 +6372,31 @@
         <v>4</v>
       </c>
       <c r="V56">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W56">
         <v>3</v>
       </c>
       <c r="X56">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y56">
         <v>10</v>
       </c>
       <c r="Z56">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA56">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB56">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC56">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD56">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE56" t="s">
         <v>178</v>
@@ -6470,31 +6470,31 @@
         <v>4</v>
       </c>
       <c r="V57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W57">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X57">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y57">
         <v>10</v>
       </c>
       <c r="Z57">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA57">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB57">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC57">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD57">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE57" t="s">
         <v>178</v>
@@ -6568,31 +6568,31 @@
         <v>4</v>
       </c>
       <c r="V58">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W58">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="X58">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y58">
         <v>10</v>
       </c>
       <c r="Z58">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA58">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB58">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC58">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD58">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE58" t="s">
         <v>178</v>
@@ -6669,28 +6669,28 @@
         <v>0</v>
       </c>
       <c r="W59">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="X59">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y59">
         <v>10</v>
       </c>
       <c r="Z59">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA59">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB59">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC59">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD59">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE59" t="s">
         <v>178</v>
@@ -6764,31 +6764,31 @@
         <v>4</v>
       </c>
       <c r="V60">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W60">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="X60">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y60">
         <v>10</v>
       </c>
       <c r="Z60">
-        <v>2783.682849755817</v>
+        <v>4306.23384085033</v>
       </c>
       <c r="AA60">
-        <v>1180.695202528009</v>
+        <v>1479.459925308819</v>
       </c>
       <c r="AB60">
-        <v>0.8161824740233883</v>
+        <v>0.6061422201693962</v>
       </c>
       <c r="AC60">
-        <v>1.096545340279757</v>
+        <v>0.9440316658385822</v>
       </c>
       <c r="AD60">
-        <v>1.282654281874478</v>
+        <v>0.9554495506517963</v>
       </c>
       <c r="AE60" t="s">
         <v>178</v>

</xml_diff>